<commit_message>
WebDriver Util Class created
</commit_message>
<xml_diff>
--- a/SDET5 Excel.xlsx
+++ b/SDET5 Excel.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Pavan</t>
   </si>
@@ -32,12 +32,6 @@
   </si>
   <si>
     <t>Padmaja</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Salary</t>
   </si>
   <si>
     <t>Urmila</t>
@@ -372,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -385,57 +379,49 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>30000</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>30000</v>
+        <v>32000</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>32000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>25000</v>
+        <v>33000</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>33000</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>40000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7">
         <v>38000</v>
       </c>
     </row>

</xml_diff>